<commit_message>
Add the new Things
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework2\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D043D3-34E3-4EAA-A28C-04A4798880F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5914A0E-E786-4F0B-9DCE-A97FAFA81A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="308">
   <si>
     <t>Si No</t>
   </si>
@@ -690,13 +690,275 @@
   </si>
   <si>
     <t>User should be able to login after entering OTP</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>//li[@title = 'Timesheets']</t>
+  </si>
+  <si>
+    <t>(//select[@class = 'form-control ng-untouched ng-pristine ng-valid'])[1]</t>
+  </si>
+  <si>
+    <t>SelectVisibleText</t>
+  </si>
+  <si>
+    <t>Day_Type</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>//input[@placeholder = 'Select In Time']</t>
+  </si>
+  <si>
+    <t>//*[@class="owl-dt-calendar-view ng-star-inserted"]/table/tbody</t>
+  </si>
+  <si>
+    <t>(//input[@class = 'owl-dt-timer-input'])[1]</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>(//input[@class = 'owl-dt-timer-input'])[2]</t>
+  </si>
+  <si>
+    <t>InTime_Second</t>
+  </si>
+  <si>
+    <t>InTime_Hour</t>
+  </si>
+  <si>
+    <t>//span[text() = "Set"]</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>(//span[@class = "owl-dt-control-button-content"])[5]</t>
+  </si>
+  <si>
+    <t>AM_Morning</t>
+  </si>
+  <si>
+    <t>//input[@placeholder = 'Select Out Time']</t>
+  </si>
+  <si>
+    <t>DateChoose</t>
+  </si>
+  <si>
+    <t>OutTime_Hour</t>
+  </si>
+  <si>
+    <t>OutTime_Second</t>
+  </si>
+  <si>
+    <t>PM_Night</t>
+  </si>
+  <si>
+    <t>ScrollDown(500)</t>
+  </si>
+  <si>
+    <t>//div[@id = "mat-select-value-1"]</t>
+  </si>
+  <si>
+    <t>clientName</t>
+  </si>
+  <si>
+    <t>Kotak Bank</t>
+  </si>
+  <si>
+    <t>VK_ENTER</t>
+  </si>
+  <si>
+    <t>mat-select-value-3</t>
+  </si>
+  <si>
+    <t>mat-select-value-5</t>
+  </si>
+  <si>
+    <t>//select[@class = "form-control ng-untouched ng-pristine ng-valid"]</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>ACTIVITY</t>
+  </si>
+  <si>
+    <t>//textarea[@class = "form-control ng-untouched ng-pristine ng-valid"]</t>
+  </si>
+  <si>
+    <t>Working on the TA module</t>
+  </si>
+  <si>
+    <t>//input[@class = "form-control ng-untouched ng-pristine"]</t>
+  </si>
+  <si>
+    <t>GetTotalWorkingHour</t>
+  </si>
+  <si>
+    <t>DisableFieldGetText</t>
+  </si>
+  <si>
+    <t>//input[@class = "form-control ng-untouched ng-pristine ng-valid"]</t>
+  </si>
+  <si>
+    <t>//button[text() = "Create Timesheet"]</t>
+  </si>
+  <si>
+    <t>//button[text() = "OK"]</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Working on TA module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,8 +986,40 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF0000C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +1029,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,12 +1058,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1081,46 +1398,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="35.6640625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1128,19 +1445,19 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>14</v>
       </c>
     </row>
@@ -1148,22 +1465,22 @@
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C3" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>19</v>
       </c>
     </row>
@@ -1171,16 +1488,16 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C4" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1188,31 +1505,31 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>140</v>
       </c>
     </row>
@@ -1220,28 +1537,28 @@
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>138</v>
       </c>
     </row>
@@ -1249,16 +1566,16 @@
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="C7" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>135</v>
       </c>
     </row>
@@ -1266,28 +1583,28 @@
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>141</v>
       </c>
     </row>
@@ -1295,16 +1612,16 @@
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="C9" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s" s="0">
         <v>135</v>
       </c>
     </row>
@@ -1312,31 +1629,31 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>137</v>
       </c>
     </row>
@@ -1344,25 +1661,25 @@
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C11" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>142</v>
       </c>
     </row>
@@ -1370,16 +1687,16 @@
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="C12" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s" s="0">
         <v>154</v>
       </c>
     </row>
@@ -1387,16 +1704,16 @@
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="C13" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s" s="0">
         <v>119</v>
       </c>
     </row>
@@ -1404,16 +1721,16 @@
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="C14" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s" s="0">
         <v>122</v>
       </c>
     </row>
@@ -1421,19 +1738,19 @@
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="C15" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -1441,16 +1758,16 @@
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" t="s" s="0">
         <v>95</v>
       </c>
     </row>
@@ -1458,31 +1775,31 @@
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s" s="0">
         <v>70</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" t="s" s="0">
         <v>144</v>
       </c>
     </row>
@@ -1490,28 +1807,28 @@
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C18" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s" s="0">
         <v>67</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="s" s="0">
         <v>145</v>
       </c>
     </row>
@@ -1519,16 +1836,16 @@
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="C19" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1536,22 +1853,22 @@
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C20" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -1559,16 +1876,16 @@
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="C21" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1576,28 +1893,28 @@
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="C22" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" t="s" s="0">
         <v>141</v>
       </c>
     </row>
@@ -1605,16 +1922,16 @@
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="C23" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1622,22 +1939,22 @@
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C24" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s" s="0">
         <v>67</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -1645,16 +1962,16 @@
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="C25" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s" s="0">
         <v>153</v>
       </c>
     </row>
@@ -1662,22 +1979,22 @@
       <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="C26" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" t="s" s="0">
         <v>76</v>
       </c>
     </row>
@@ -1685,16 +2002,16 @@
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="C27" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s" s="0">
         <v>87</v>
       </c>
     </row>
@@ -1702,22 +2019,22 @@
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>81</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" t="s" s="0">
         <v>83</v>
       </c>
     </row>
@@ -1725,17 +2042,17 @@
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s" s="0">
         <v>79</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="H29" t="s">
+      <c r="H29" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1743,31 +2060,31 @@
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C30" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="s" s="0">
         <v>81</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" t="s" s="0">
         <v>157</v>
       </c>
     </row>
@@ -1775,22 +2092,22 @@
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="C31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" t="s" s="0">
         <v>81</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" t="s" s="0">
         <v>80</v>
       </c>
     </row>
@@ -1798,16 +2115,16 @@
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="C32" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s" s="0">
         <v>121</v>
       </c>
     </row>
@@ -1815,16 +2132,16 @@
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="C33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="C33" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s" s="0">
         <v>96</v>
       </c>
     </row>
@@ -1832,16 +2149,16 @@
       <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="C34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C34" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" t="s" s="0">
         <v>87</v>
       </c>
     </row>
@@ -1849,16 +2166,16 @@
       <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" t="s" s="0">
         <v>123</v>
       </c>
     </row>
@@ -1866,17 +2183,17 @@
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s" s="0">
         <v>79</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="H36" t="s">
+      <c r="H36" t="s" s="0">
         <v>147</v>
       </c>
     </row>
@@ -1884,25 +2201,25 @@
       <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="C37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="C37" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s" s="0">
         <v>70</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" t="s" s="0">
         <v>146</v>
       </c>
     </row>
@@ -1910,31 +2227,31 @@
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" t="s" s="0">
         <v>137</v>
       </c>
     </row>
@@ -1942,22 +2259,22 @@
       <c r="A39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -1965,16 +2282,16 @@
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="C40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" t="s" s="0">
         <v>95</v>
       </c>
     </row>
@@ -1982,16 +2299,16 @@
       <c r="A41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" t="s" s="0">
         <v>152</v>
       </c>
     </row>
@@ -1999,7 +2316,7 @@
       <c r="A42" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>149</v>
       </c>
     </row>
@@ -2012,63 +2329,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE73440-ADC0-400F-94D2-AEBDBE56EBE3}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="59.88671875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.5546875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.88671875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.33203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="47.21875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>164</v>
       </c>
     </row>
@@ -2076,25 +2393,25 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>166</v>
       </c>
     </row>
@@ -2102,28 +2419,28 @@
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>172</v>
       </c>
     </row>
@@ -2131,25 +2448,25 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>173</v>
       </c>
     </row>
@@ -2157,37 +2474,37 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>215</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>174</v>
       </c>
     </row>
@@ -2195,34 +2512,34 @@
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>175</v>
       </c>
     </row>
@@ -2230,25 +2547,25 @@
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="D7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>176</v>
       </c>
     </row>
@@ -2256,34 +2573,34 @@
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>177</v>
       </c>
     </row>
@@ -2291,25 +2608,25 @@
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="D9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>178</v>
       </c>
     </row>
@@ -2317,34 +2634,34 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>179</v>
       </c>
     </row>
@@ -2352,31 +2669,31 @@
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>180</v>
       </c>
     </row>
@@ -2384,25 +2701,25 @@
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="D12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" t="s" s="0">
         <v>181</v>
       </c>
     </row>
@@ -2410,25 +2727,25 @@
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="D13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" t="s" s="0">
         <v>182</v>
       </c>
     </row>
@@ -2436,28 +2753,28 @@
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="D14" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" t="s" s="0">
         <v>183</v>
       </c>
     </row>
@@ -2465,28 +2782,28 @@
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="D15" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" t="s" s="0">
         <v>184</v>
       </c>
     </row>
@@ -2494,25 +2811,25 @@
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="D16" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" t="s" s="0">
         <v>185</v>
       </c>
     </row>
@@ -2520,34 +2837,34 @@
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" t="s" s="0">
         <v>186</v>
       </c>
     </row>
@@ -2555,34 +2872,34 @@
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" t="s" s="0">
         <v>187</v>
       </c>
     </row>
@@ -2590,25 +2907,25 @@
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="D19" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" t="s" s="0">
         <v>188</v>
       </c>
     </row>
@@ -2616,31 +2933,31 @@
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" t="s" s="0">
         <v>189</v>
       </c>
     </row>
@@ -2648,25 +2965,25 @@
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="D21" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" t="s" s="0">
         <v>190</v>
       </c>
     </row>
@@ -2674,34 +2991,34 @@
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" t="s" s="0">
         <v>191</v>
       </c>
     </row>
@@ -2709,25 +3026,25 @@
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="D23" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" t="s" s="0">
         <v>192</v>
       </c>
     </row>
@@ -2735,31 +3052,31 @@
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" t="s" s="0">
         <v>193</v>
       </c>
     </row>
@@ -2767,25 +3084,25 @@
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="D25" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" t="s" s="0">
         <v>194</v>
       </c>
     </row>
@@ -2793,31 +3110,31 @@
       <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" t="s" s="0">
         <v>195</v>
       </c>
     </row>
@@ -2825,25 +3142,25 @@
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="D27" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" t="s" s="0">
         <v>196</v>
       </c>
     </row>
@@ -2851,31 +3168,31 @@
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" t="s" s="0">
         <v>197</v>
       </c>
     </row>
@@ -2883,26 +3200,26 @@
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>12</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="H29" t="s">
+      <c r="H29" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" t="s" s="0">
         <v>198</v>
       </c>
     </row>
@@ -2910,34 +3227,34 @@
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E30" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" t="s" s="0">
         <v>199</v>
       </c>
     </row>
@@ -2945,31 +3262,31 @@
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" t="s" s="0">
         <v>200</v>
       </c>
     </row>
@@ -2977,25 +3294,25 @@
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="D32" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L32" t="s" s="0">
         <v>201</v>
       </c>
     </row>
@@ -3003,25 +3320,25 @@
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="D33" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" t="s" s="0">
         <v>202</v>
       </c>
     </row>
@@ -3029,25 +3346,25 @@
       <c r="A34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="D34" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" t="s" s="0">
         <v>203</v>
       </c>
     </row>
@@ -3055,25 +3372,25 @@
       <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="D35" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35" t="s" s="0">
         <v>204</v>
       </c>
     </row>
@@ -3081,26 +3398,26 @@
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>12</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="H36" t="s">
+      <c r="H36" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L36" t="s" s="0">
         <v>205</v>
       </c>
     </row>
@@ -3108,31 +3425,31 @@
       <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B37" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D37" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" t="s" s="0">
         <v>206</v>
       </c>
     </row>
@@ -3140,34 +3457,34 @@
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" t="s" s="0">
         <v>207</v>
       </c>
     </row>
@@ -3175,31 +3492,31 @@
       <c r="A39" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B39" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" t="s" s="0">
         <v>208</v>
       </c>
     </row>
@@ -3207,96 +3524,1536 @@
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="D40" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" t="s" s="0">
         <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="A41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="D41" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H41" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41" t="s" s="0">
         <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F42" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="H42" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J42" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K42" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L42" t="s" s="0">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="J43" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K43" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L43" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J44" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K44" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L44" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J45" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K45" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L45" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="H46" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J46" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K46" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L46" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J47" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K47" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L47" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F48" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="J48" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K48" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L48" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J49" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K49" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L49" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F50" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J50" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K50" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L50" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F51" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="G51" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J51" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K51" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L51" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J52" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K52" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L52" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F53" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J53" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K53" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L53" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F54" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="G54" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J54" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K54" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L54" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H55" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="J55" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="K55" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="L55" t="s" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J56" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K56" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L56" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F57" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="H57" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J57" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K57" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L57" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J58" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K58" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L58" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F59" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="H59" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J59" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K59" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L59" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H60" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J60" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K60" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L60" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F61" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="J61" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K61" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L61" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H62" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J62" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K62" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L62" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F63" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J63" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K63" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L63" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="G64" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J64" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K64" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L64" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H65" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J65" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K65" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L65" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E66" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F66" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J66" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K66" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L66" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E67" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F67" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="G67" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J67" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K67" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L67" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="D68" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E68" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="J68" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="K68" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="L68" t="s" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D69" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H69" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J69" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K69" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L69" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D70" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F70" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="H70" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J70" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K70" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L70" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D71" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H71" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J71" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K71" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L71" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="D72" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="J72" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="K72" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="L72" t="s" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D73" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="J73" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K73" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L73" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D74" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E74" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F74" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J74" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K74" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L74" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D75" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="J75" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K75" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L75" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C76" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D76" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H76" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J76" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K76" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L76" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C77" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D77" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E77" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="F77" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J77" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K77" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L77" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C78" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D78" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="J78" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K78" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L78" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D79" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H79" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J79" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K79" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L79" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C80" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D80" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E80" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="F80" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J80" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K80" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L80" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C81" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D81" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H81" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="J81" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K81" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L81" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C82" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D82" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E82" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F82" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="G82" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J82" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K82" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L82" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C83" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D83" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="H83" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J83" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K83" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L83" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C84" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D84" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E84" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F84" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="G84" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J84" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K84" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L84" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C85" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D85" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F85" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="J85" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K85" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L85" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B86" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C86" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D86" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="E86" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F86" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J86" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K86" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L86" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B87" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C87" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D87" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="H87" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J87" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K87" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L87" t="s" s="0">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B88" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C88" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D88" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="E88" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F88" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J88" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="K88" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="L88" t="s" s="0">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B700F1-826A-4855-8A91-C6D9EF1F36AA}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.6640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.6640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5546875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="G1" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="L1" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="N1" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3305,14 +5062,38 @@
       <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="F2" t="b">
+      <c r="F2" t="b" s="0">
         <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>